<commit_message>
Fix primi due articoli
</commit_message>
<xml_diff>
--- a/download/Calcolatore-BOT.xlsx
+++ b/download/Calcolatore-BOT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sasadangelo/github.com/sasadangelo/investire/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6901A762-48CF-C044-A708-589A903EA15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734A56DA-79F1-8940-A4B5-AE5C1858A40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12000" yWindow="500" windowWidth="25600" windowHeight="14480" xr2:uid="{384A719B-2758-B34C-9A5E-16DC06482511}"/>
+    <workbookView xWindow="2560" yWindow="1120" windowWidth="25600" windowHeight="14480" xr2:uid="{384A719B-2758-B34C-9A5E-16DC06482511}"/>
   </bookViews>
   <sheets>
     <sheet name="BOT Calcolatore" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="79">
   <si>
     <t>ISIN</t>
   </si>
@@ -43,12 +43,6 @@
     <t>Nome</t>
   </si>
   <si>
-    <t>IT0005532988</t>
-  </si>
-  <si>
-    <t>BOT 14FB24 ANN</t>
-  </si>
-  <si>
     <t>Data Emissione</t>
   </si>
   <si>
@@ -122,9 +116,6 @@
   </si>
   <si>
     <t>Costi Fissi + Bollo (EUR)</t>
-  </si>
-  <si>
-    <t>Costi Fissi + Commissioni + Bollo (EUR)</t>
   </si>
   <si>
     <t>Il prezzo di emissione di un titolo rappresenta il prezzo iniziale al quale il titolo viene messo in vendita sul mercato, ovvero il prezzo al quale gli investitori possono acquistare il titolo alla sua emissione. In altre parole, il prezzo di emissione rappresenta il valore nominale del titolo al momento della sua prima offerta al pubblico. Questo prezzo di emissione viene fissato dal Tesoro italiano e può variare a seconda delle condizioni di mercato, della durata del titolo e del tasso di interesse offerto.</t>
@@ -304,6 +295,206 @@
   <si>
     <t>Importo Totale Pagato (EUR)</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">È la durata residua del BOT, ossia il numero di giorni dalla Data di Acquisto alla Data di Scadenza. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Durata Residua</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Data Acquisto </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Data Scadenza</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">È la durata già trascorsa del BOT, ossia il numero di giorni dalla Data di Emissione alla Data di Acquisto. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Durata Trascorsa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Data Emissione </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Data Acquisto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">È il prodotto tra il Prezzo Pagato per la Quantità di BOT Acquistati. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Importo Secco = Prezzo Acquisto * Quantità</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Immaginando una retta di interpolazione che unisce, nel tempo, il Prezzo di Emissione alla Data di Emissione e 100 alla Data di Scadenza, il Prezzo Teorico è il punto della retta con ascisse la Data di Acquisto. Il calcolo di questo Prezzo è importante per capire se l'investimento genera o meno ulteriori plusvalenze da tassare o minusvalenze che possono compensare plusvalenze di altri investimenti. La formula usata è </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prezzo Teorico = Prezzo Emissione + (100 - Prezzo Emission) * (Durata Trascorsa/Durata)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Costi Fissi</t>
+  </si>
+  <si>
+    <t>Costi Fissi + Commissioni</t>
+  </si>
+  <si>
+    <t>IT0005545469</t>
+  </si>
+  <si>
+    <t>BOT 14MG24 ANN</t>
+  </si>
 </sst>
 </file>
 
@@ -313,7 +504,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -341,6 +532,13 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -799,7 +997,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -861,7 +1059,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -871,33 +1077,45 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -916,14 +1134,53 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -934,6 +1191,57 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -943,72 +1251,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1032,27 +1274,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1368,10 +1589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C8A721-BA1D-A549-9B83-DE9858641FEB}">
-  <dimension ref="B1:H117"/>
+  <dimension ref="B1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1385,179 +1606,179 @@
   <sheetData>
     <row r="1" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="73" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="75"/>
+      <c r="B2" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="65"/>
     </row>
     <row r="3" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="55"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="57"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="76"/>
     </row>
     <row r="4" spans="2:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="91" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="79"/>
+      <c r="E4" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="69"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <v>0.125</v>
       </c>
-      <c r="C5" s="92"/>
+      <c r="C5" s="67"/>
       <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="69"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="77"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="79"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="94"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E6" s="7">
-        <v>44971</v>
-      </c>
-      <c r="F6" s="79"/>
+        <v>45060</v>
+      </c>
+      <c r="F6" s="69"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="64"/>
-      <c r="C7" s="92"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="8">
         <v>96.876999999999995</v>
       </c>
-      <c r="F7" s="79"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="64"/>
-      <c r="C8" s="93"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E8" s="7">
         <v>45336</v>
       </c>
-      <c r="F8" s="79"/>
+      <c r="F8" s="69"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="80"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="82"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="73"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="64"/>
-      <c r="C10" s="91" t="s">
-        <v>9</v>
+      <c r="B10" s="70"/>
+      <c r="C10" s="66" t="s">
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E10" s="7">
         <v>44986</v>
       </c>
-      <c r="F10" s="79"/>
+      <c r="F10" s="69"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="64"/>
-      <c r="C11" s="92"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E11" s="8">
-        <v>96.846000000000004</v>
-      </c>
-      <c r="F11" s="79"/>
+        <v>97.161000000000001</v>
+      </c>
+      <c r="F11" s="69"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="64"/>
-      <c r="C12" s="92"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E12" s="8">
-        <v>0.24</v>
-      </c>
-      <c r="F12" s="79"/>
+        <v>0.15</v>
+      </c>
+      <c r="F12" s="69"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="64"/>
-      <c r="C13" s="92"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="67"/>
       <c r="D13" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E13" s="28">
         <v>3</v>
       </c>
-      <c r="F13" s="79"/>
+      <c r="F13" s="69"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="64"/>
-      <c r="C14" s="92"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="79"/>
+        <v>41</v>
+      </c>
+      <c r="F14" s="69"/>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="64"/>
-      <c r="C15" s="92"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="67"/>
       <c r="D15" s="1" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="E15" s="28">
-        <v>3.5</v>
-      </c>
-      <c r="F15" s="79"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="69"/>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="64"/>
-      <c r="C16" s="93"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="68"/>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E16" s="28">
         <v>5000</v>
       </c>
-      <c r="F16" s="79"/>
+      <c r="F16" s="69"/>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
@@ -1571,10 +1792,10 @@
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="11"/>
       <c r="C18" s="24" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E18" s="8">
         <v>0</v>
@@ -1592,11 +1813,11 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
-      <c r="C20" s="61" t="s">
-        <v>47</v>
+      <c r="C20" s="81" t="s">
+        <v>44</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E20" s="4">
         <f>E16/100</f>
@@ -1606,21 +1827,21 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="11"/>
-      <c r="C21" s="62"/>
+      <c r="C21" s="82"/>
       <c r="D21" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E21" s="20">
         <f>E8-E6</f>
-        <v>365</v>
+        <v>276</v>
       </c>
       <c r="F21" s="13"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="11"/>
-      <c r="C22" s="62"/>
+      <c r="C22" s="82"/>
       <c r="D22" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E22" s="20">
         <f>E8-E10</f>
@@ -1630,25 +1851,25 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="11"/>
-      <c r="C23" s="62"/>
+      <c r="C23" s="82"/>
       <c r="D23" s="19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E23" s="20">
         <f>E10-E6</f>
-        <v>15</v>
+        <v>-74</v>
       </c>
       <c r="F23" s="13"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="11"/>
-      <c r="C24" s="63"/>
+      <c r="C24" s="83"/>
       <c r="D24" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E24" s="31">
         <f>E7+(100-E7)*(E23/E21)</f>
-        <v>97.005342465753415</v>
+        <v>96.039673913043472</v>
       </c>
       <c r="F24" s="13"/>
     </row>
@@ -1660,70 +1881,70 @@
       <c r="F25" s="13"/>
     </row>
     <row r="26" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="64"/>
-      <c r="C26" s="95" t="s">
-        <v>49</v>
+      <c r="B26" s="70"/>
+      <c r="C26" s="78" t="s">
+        <v>46</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E26" s="4">
         <f>E11*E20</f>
-        <v>4842.3</v>
-      </c>
-      <c r="F26" s="79"/>
+        <v>4858.05</v>
+      </c>
+      <c r="F26" s="69"/>
       <c r="H26" s="27"/>
     </row>
     <row r="27" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="64"/>
-      <c r="C27" s="96"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="79"/>
       <c r="D27" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E27" s="29">
         <f>MIN(MAX(E26*E12/100,E13),E14)</f>
-        <v>11.62152</v>
-      </c>
-      <c r="F27" s="79"/>
+        <v>7.2870749999999997</v>
+      </c>
+      <c r="F27" s="69"/>
       <c r="H27" s="27"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="64"/>
-      <c r="C28" s="96"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="79"/>
       <c r="D28" s="10" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="E28" s="29">
         <f>E27+E15</f>
-        <v>15.12152</v>
-      </c>
-      <c r="F28" s="79"/>
+        <v>7.2870749999999997</v>
+      </c>
+      <c r="F28" s="69"/>
       <c r="H28" s="27"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="64"/>
-      <c r="C29" s="96"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="79"/>
       <c r="D29" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E29" s="29">
         <f>(100-E7)*(E22/E21)*E20*B5</f>
-        <v>18.716609589041123</v>
-      </c>
-      <c r="F29" s="79"/>
+        <v>24.752038043478301</v>
+      </c>
+      <c r="F29" s="69"/>
       <c r="H29" s="27"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="64"/>
-      <c r="C30" s="97"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="80"/>
       <c r="D30" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E30" s="30">
         <f>E26+E28+E29</f>
-        <v>4876.1381295890405</v>
-      </c>
-      <c r="F30" s="79"/>
+        <v>4890.0891130434784</v>
+      </c>
+      <c r="F30" s="69"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="11"/>
@@ -1734,37 +1955,37 @@
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="11"/>
-      <c r="C32" s="61" t="s">
-        <v>50</v>
+      <c r="C32" s="81" t="s">
+        <v>47</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E32" s="26">
         <f>(E26+E27+E15)/E20-E24+E7</f>
-        <v>97.020087934246575</v>
+        <v>98.144067586956524</v>
       </c>
       <c r="F32" s="13"/>
       <c r="H32" s="27"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" s="11"/>
-      <c r="C33" s="62"/>
+      <c r="C33" s="82"/>
       <c r="D33" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E33" s="29">
         <f>(E7-E32)*E20</f>
-        <v>-7.1543967123290031</v>
+        <v>-63.353379347826433</v>
       </c>
       <c r="F33" s="13"/>
       <c r="H33" s="27"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" s="11"/>
-      <c r="C34" s="62"/>
+      <c r="C34" s="82"/>
       <c r="D34" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E34" s="4">
         <f>IF(E18&gt;E33,0,E18-E33)</f>
@@ -1774,9 +1995,9 @@
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" s="11"/>
-      <c r="C35" s="62"/>
+      <c r="C35" s="82"/>
       <c r="D35" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E35" s="4">
         <f>E34*B5</f>
@@ -1786,21 +2007,21 @@
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" s="11"/>
-      <c r="C36" s="62"/>
+      <c r="C36" s="82"/>
       <c r="D36" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E36" s="29">
         <f>IF(E18-E33&lt;0,0,E18-E33)</f>
-        <v>7.1543967123290031</v>
+        <v>63.353379347826433</v>
       </c>
       <c r="F36" s="13"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" s="11"/>
-      <c r="C37" s="63"/>
+      <c r="C37" s="83"/>
       <c r="D37" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E37" s="9">
         <f>E16-E35</f>
@@ -1809,792 +2030,887 @@
       <c r="F37" s="13"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="80"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="81"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="82"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="73"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="64"/>
-      <c r="C39" s="61" t="s">
-        <v>15</v>
+      <c r="B39" s="70"/>
+      <c r="C39" s="81" t="s">
+        <v>13</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E39" s="4">
         <f>100-E11</f>
-        <v>3.1539999999999964</v>
-      </c>
-      <c r="F39" s="79"/>
+        <v>2.8389999999999986</v>
+      </c>
+      <c r="F39" s="69"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="64"/>
-      <c r="C40" s="62"/>
+      <c r="B40" s="70"/>
+      <c r="C40" s="82"/>
       <c r="D40" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E40" s="29">
         <f>E16-E26</f>
-        <v>157.69999999999982</v>
-      </c>
-      <c r="F40" s="79"/>
+        <v>141.94999999999982</v>
+      </c>
+      <c r="F40" s="69"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B41" s="64"/>
-      <c r="C41" s="62"/>
+      <c r="B41" s="70"/>
+      <c r="C41" s="82"/>
       <c r="D41" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E41" s="29">
         <f>E42/E20</f>
-        <v>2.4772374082191893</v>
-      </c>
-      <c r="F41" s="79"/>
+        <v>2.1982177391304321</v>
+      </c>
+      <c r="F41" s="69"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="64"/>
-      <c r="C42" s="63"/>
+      <c r="B42" s="70"/>
+      <c r="C42" s="83"/>
       <c r="D42" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E42" s="30">
         <f>E37-E30</f>
-        <v>123.86187041095945</v>
-      </c>
-      <c r="F42" s="79"/>
+        <v>109.91088695652161</v>
+      </c>
+      <c r="F42" s="69"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B43" s="80"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="82"/>
+      <c r="B43" s="71"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="72"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="73"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B44" s="64"/>
-      <c r="C44" s="61" t="s">
-        <v>18</v>
+      <c r="B44" s="70"/>
+      <c r="C44" s="81" t="s">
+        <v>16</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E44" s="30">
         <f>(E39*100/E11)*(E21/E22)</f>
-        <v>3.3962904286923825</v>
-      </c>
-      <c r="F44" s="79"/>
+        <v>2.304169662430692</v>
+      </c>
+      <c r="F44" s="69"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B45" s="64"/>
-      <c r="C45" s="63"/>
+      <c r="B45" s="70"/>
+      <c r="C45" s="83"/>
       <c r="D45" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E45" s="30">
         <f>(E41*100/E11)*(E21/E22)</f>
-        <v>2.6675389027056333</v>
-      </c>
-      <c r="F45" s="79"/>
+        <v>1.784102369116354</v>
+      </c>
+      <c r="F45" s="69"/>
     </row>
     <row r="46" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="76"/>
-      <c r="C46" s="77"/>
-      <c r="D46" s="77"/>
-      <c r="E46" s="77"/>
-      <c r="F46" s="78"/>
+      <c r="B46" s="86"/>
+      <c r="C46" s="87"/>
+      <c r="D46" s="87"/>
+      <c r="E46" s="87"/>
+      <c r="F46" s="88"/>
     </row>
     <row r="47" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="C49" s="74"/>
-      <c r="D49" s="74"/>
-      <c r="E49" s="74"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="74"/>
-      <c r="H49" s="75"/>
+      <c r="B49" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="64"/>
+      <c r="D49" s="64"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="64"/>
+      <c r="G49" s="64"/>
+      <c r="H49" s="65"/>
     </row>
     <row r="50" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="55"/>
-      <c r="C50" s="56"/>
-      <c r="D50" s="56"/>
-      <c r="E50" s="56"/>
-      <c r="F50" s="56"/>
-      <c r="G50" s="56"/>
-      <c r="H50" s="57"/>
+      <c r="B50" s="74"/>
+      <c r="C50" s="75"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="75"/>
+      <c r="F50" s="75"/>
+      <c r="G50" s="75"/>
+      <c r="H50" s="76"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B51" s="58"/>
-      <c r="C51" s="59"/>
-      <c r="D51" s="59"/>
-      <c r="E51" s="59"/>
-      <c r="F51" s="59"/>
-      <c r="G51" s="59"/>
-      <c r="H51" s="60"/>
+      <c r="B51" s="94"/>
+      <c r="C51" s="95"/>
+      <c r="D51" s="95"/>
+      <c r="E51" s="95"/>
+      <c r="F51" s="95"/>
+      <c r="G51" s="95"/>
+      <c r="H51" s="96"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B52" s="87" t="s">
-        <v>48</v>
-      </c>
-      <c r="C52" s="53"/>
-      <c r="D52" s="53"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="54"/>
+      <c r="B52" s="101" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="47"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="48"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B53" s="88"/>
-      <c r="C53" s="68"/>
-      <c r="D53" s="68"/>
-      <c r="E53" s="68"/>
-      <c r="F53" s="68"/>
-      <c r="G53" s="68"/>
-      <c r="H53" s="69"/>
+      <c r="B53" s="102"/>
+      <c r="C53" s="61"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="61"/>
+      <c r="F53" s="61"/>
+      <c r="G53" s="61"/>
+      <c r="H53" s="62"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B54" s="88"/>
-      <c r="C54" s="68"/>
-      <c r="D54" s="68"/>
-      <c r="E54" s="68"/>
-      <c r="F54" s="68"/>
-      <c r="G54" s="68"/>
-      <c r="H54" s="69"/>
+      <c r="B54" s="102"/>
+      <c r="C54" s="61"/>
+      <c r="D54" s="61"/>
+      <c r="E54" s="61"/>
+      <c r="F54" s="61"/>
+      <c r="G54" s="61"/>
+      <c r="H54" s="62"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="88"/>
-      <c r="C55" s="68"/>
-      <c r="D55" s="68"/>
-      <c r="E55" s="68"/>
-      <c r="F55" s="68"/>
-      <c r="G55" s="68"/>
-      <c r="H55" s="69"/>
+      <c r="B55" s="102"/>
+      <c r="C55" s="61"/>
+      <c r="D55" s="61"/>
+      <c r="E55" s="61"/>
+      <c r="F55" s="61"/>
+      <c r="G55" s="61"/>
+      <c r="H55" s="62"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="C56" s="47"/>
-      <c r="D56" s="47"/>
-      <c r="E56" s="47"/>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="48"/>
+      <c r="B56" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="53"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="53"/>
+      <c r="F56" s="53"/>
+      <c r="G56" s="53"/>
+      <c r="H56" s="54"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="49"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="50"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="50"/>
-      <c r="G57" s="50"/>
-      <c r="H57" s="51"/>
+      <c r="B57" s="55"/>
+      <c r="C57" s="56"/>
+      <c r="D57" s="56"/>
+      <c r="E57" s="56"/>
+      <c r="F57" s="56"/>
+      <c r="G57" s="56"/>
+      <c r="H57" s="57"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58" s="21"/>
-      <c r="C58" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="35"/>
-      <c r="G58" s="35"/>
-      <c r="H58" s="36"/>
+      <c r="C58" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="38"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B59" s="22"/>
-      <c r="C59" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D59" s="35"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="35"/>
-      <c r="H59" s="36"/>
+      <c r="C59" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="38"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" s="23"/>
-      <c r="C60" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="D60" s="35"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="35"/>
-      <c r="G60" s="35"/>
-      <c r="H60" s="36"/>
+      <c r="C60" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" s="37"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="38"/>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B61" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="C61" s="47"/>
-      <c r="D61" s="47"/>
-      <c r="E61" s="47"/>
-      <c r="F61" s="47"/>
-      <c r="G61" s="47"/>
-      <c r="H61" s="48"/>
+      <c r="B61" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C61" s="53"/>
+      <c r="D61" s="53"/>
+      <c r="E61" s="53"/>
+      <c r="F61" s="53"/>
+      <c r="G61" s="53"/>
+      <c r="H61" s="54"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="49"/>
-      <c r="C62" s="50"/>
-      <c r="D62" s="50"/>
-      <c r="E62" s="50"/>
-      <c r="F62" s="50"/>
-      <c r="G62" s="50"/>
-      <c r="H62" s="51"/>
+      <c r="B62" s="55"/>
+      <c r="C62" s="56"/>
+      <c r="D62" s="56"/>
+      <c r="E62" s="56"/>
+      <c r="F62" s="56"/>
+      <c r="G62" s="56"/>
+      <c r="H62" s="57"/>
     </row>
     <row r="63" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="72" t="s">
+      <c r="B63" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C63" s="70" t="s">
-        <v>39</v>
-      </c>
-      <c r="D63" s="70"/>
-      <c r="E63" s="70"/>
-      <c r="F63" s="70"/>
-      <c r="G63" s="70"/>
-      <c r="H63" s="71"/>
+      <c r="C63" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="D63" s="84"/>
+      <c r="E63" s="84"/>
+      <c r="F63" s="84"/>
+      <c r="G63" s="84"/>
+      <c r="H63" s="85"/>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B64" s="72"/>
-      <c r="C64" s="70"/>
-      <c r="D64" s="70"/>
-      <c r="E64" s="70"/>
-      <c r="F64" s="70"/>
-      <c r="G64" s="70"/>
-      <c r="H64" s="71"/>
+      <c r="B64" s="39"/>
+      <c r="C64" s="84"/>
+      <c r="D64" s="84"/>
+      <c r="E64" s="84"/>
+      <c r="F64" s="84"/>
+      <c r="G64" s="84"/>
+      <c r="H64" s="85"/>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B65" s="72"/>
-      <c r="C65" s="70"/>
-      <c r="D65" s="70"/>
-      <c r="E65" s="70"/>
-      <c r="F65" s="70"/>
-      <c r="G65" s="70"/>
-      <c r="H65" s="71"/>
+      <c r="B65" s="39"/>
+      <c r="C65" s="84"/>
+      <c r="D65" s="84"/>
+      <c r="E65" s="84"/>
+      <c r="F65" s="84"/>
+      <c r="G65" s="84"/>
+      <c r="H65" s="85"/>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B66" s="72"/>
-      <c r="C66" s="70"/>
-      <c r="D66" s="70"/>
-      <c r="E66" s="70"/>
-      <c r="F66" s="70"/>
-      <c r="G66" s="70"/>
-      <c r="H66" s="71"/>
+      <c r="B66" s="39"/>
+      <c r="C66" s="84"/>
+      <c r="D66" s="84"/>
+      <c r="E66" s="84"/>
+      <c r="F66" s="84"/>
+      <c r="G66" s="84"/>
+      <c r="H66" s="85"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C67" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="D67" s="53"/>
-      <c r="E67" s="53"/>
-      <c r="F67" s="53"/>
-      <c r="G67" s="53"/>
-      <c r="H67" s="54"/>
+      <c r="C67" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="D67" s="47"/>
+      <c r="E67" s="47"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="47"/>
+      <c r="H67" s="48"/>
     </row>
     <row r="68" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="72" t="s">
-        <v>4</v>
-      </c>
-      <c r="C68" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="D68" s="70"/>
-      <c r="E68" s="70"/>
-      <c r="F68" s="70"/>
-      <c r="G68" s="70"/>
-      <c r="H68" s="71"/>
+      <c r="B68" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" s="84" t="s">
+        <v>38</v>
+      </c>
+      <c r="D68" s="84"/>
+      <c r="E68" s="84"/>
+      <c r="F68" s="84"/>
+      <c r="G68" s="84"/>
+      <c r="H68" s="85"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B69" s="72"/>
-      <c r="C69" s="70"/>
-      <c r="D69" s="70"/>
-      <c r="E69" s="70"/>
-      <c r="F69" s="70"/>
-      <c r="G69" s="70"/>
-      <c r="H69" s="71"/>
+      <c r="B69" s="39"/>
+      <c r="C69" s="84"/>
+      <c r="D69" s="84"/>
+      <c r="E69" s="84"/>
+      <c r="F69" s="84"/>
+      <c r="G69" s="84"/>
+      <c r="H69" s="85"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B70" s="72"/>
-      <c r="C70" s="70"/>
-      <c r="D70" s="70"/>
-      <c r="E70" s="70"/>
-      <c r="F70" s="70"/>
-      <c r="G70" s="70"/>
-      <c r="H70" s="71"/>
+      <c r="B70" s="39"/>
+      <c r="C70" s="84"/>
+      <c r="D70" s="84"/>
+      <c r="E70" s="84"/>
+      <c r="F70" s="84"/>
+      <c r="G70" s="84"/>
+      <c r="H70" s="85"/>
     </row>
     <row r="71" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="72" t="s">
-        <v>24</v>
-      </c>
-      <c r="C71" s="89" t="s">
-        <v>30</v>
-      </c>
-      <c r="D71" s="89"/>
-      <c r="E71" s="89"/>
-      <c r="F71" s="89"/>
-      <c r="G71" s="89"/>
-      <c r="H71" s="90"/>
+      <c r="B71" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C71" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="D71" s="103"/>
+      <c r="E71" s="103"/>
+      <c r="F71" s="103"/>
+      <c r="G71" s="103"/>
+      <c r="H71" s="104"/>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B72" s="72"/>
-      <c r="C72" s="89"/>
-      <c r="D72" s="89"/>
-      <c r="E72" s="89"/>
-      <c r="F72" s="89"/>
-      <c r="G72" s="89"/>
-      <c r="H72" s="90"/>
+      <c r="B72" s="39"/>
+      <c r="C72" s="103"/>
+      <c r="D72" s="103"/>
+      <c r="E72" s="103"/>
+      <c r="F72" s="103"/>
+      <c r="G72" s="103"/>
+      <c r="H72" s="104"/>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B73" s="72"/>
-      <c r="C73" s="89"/>
-      <c r="D73" s="89"/>
-      <c r="E73" s="89"/>
-      <c r="F73" s="89"/>
-      <c r="G73" s="89"/>
-      <c r="H73" s="90"/>
+      <c r="B73" s="39"/>
+      <c r="C73" s="103"/>
+      <c r="D73" s="103"/>
+      <c r="E73" s="103"/>
+      <c r="F73" s="103"/>
+      <c r="G73" s="103"/>
+      <c r="H73" s="104"/>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B74" s="72"/>
-      <c r="C74" s="89"/>
-      <c r="D74" s="89"/>
-      <c r="E74" s="89"/>
-      <c r="F74" s="89"/>
-      <c r="G74" s="89"/>
-      <c r="H74" s="90"/>
+      <c r="B74" s="39"/>
+      <c r="C74" s="103"/>
+      <c r="D74" s="103"/>
+      <c r="E74" s="103"/>
+      <c r="F74" s="103"/>
+      <c r="G74" s="103"/>
+      <c r="H74" s="104"/>
     </row>
     <row r="75" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="D75" s="53"/>
-      <c r="E75" s="53"/>
-      <c r="F75" s="53"/>
-      <c r="G75" s="53"/>
-      <c r="H75" s="54"/>
+      <c r="B75" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D75" s="47"/>
+      <c r="E75" s="47"/>
+      <c r="F75" s="47"/>
+      <c r="G75" s="47"/>
+      <c r="H75" s="48"/>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B76" s="44"/>
-      <c r="C76" s="67"/>
-      <c r="D76" s="68"/>
-      <c r="E76" s="68"/>
-      <c r="F76" s="68"/>
-      <c r="G76" s="68"/>
-      <c r="H76" s="69"/>
+      <c r="B76" s="51"/>
+      <c r="C76" s="60"/>
+      <c r="D76" s="61"/>
+      <c r="E76" s="61"/>
+      <c r="F76" s="61"/>
+      <c r="G76" s="61"/>
+      <c r="H76" s="62"/>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B77" s="44"/>
-      <c r="C77" s="67"/>
-      <c r="D77" s="68"/>
-      <c r="E77" s="68"/>
-      <c r="F77" s="68"/>
-      <c r="G77" s="68"/>
-      <c r="H77" s="69"/>
+      <c r="B77" s="51"/>
+      <c r="C77" s="60"/>
+      <c r="D77" s="61"/>
+      <c r="E77" s="61"/>
+      <c r="F77" s="61"/>
+      <c r="G77" s="61"/>
+      <c r="H77" s="62"/>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B78" s="44"/>
-      <c r="C78" s="67"/>
-      <c r="D78" s="68"/>
-      <c r="E78" s="68"/>
-      <c r="F78" s="68"/>
-      <c r="G78" s="68"/>
-      <c r="H78" s="69"/>
+      <c r="B78" s="51"/>
+      <c r="C78" s="60"/>
+      <c r="D78" s="61"/>
+      <c r="E78" s="61"/>
+      <c r="F78" s="61"/>
+      <c r="G78" s="61"/>
+      <c r="H78" s="62"/>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B79" s="44"/>
-      <c r="C79" s="67"/>
-      <c r="D79" s="68"/>
-      <c r="E79" s="68"/>
-      <c r="F79" s="68"/>
-      <c r="G79" s="68"/>
-      <c r="H79" s="69"/>
+      <c r="B79" s="51"/>
+      <c r="C79" s="60"/>
+      <c r="D79" s="61"/>
+      <c r="E79" s="61"/>
+      <c r="F79" s="61"/>
+      <c r="G79" s="61"/>
+      <c r="H79" s="62"/>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B80" s="44"/>
-      <c r="C80" s="67"/>
-      <c r="D80" s="68"/>
-      <c r="E80" s="68"/>
-      <c r="F80" s="68"/>
-      <c r="G80" s="68"/>
-      <c r="H80" s="69"/>
+      <c r="B80" s="51"/>
+      <c r="C80" s="60"/>
+      <c r="D80" s="61"/>
+      <c r="E80" s="61"/>
+      <c r="F80" s="61"/>
+      <c r="G80" s="61"/>
+      <c r="H80" s="62"/>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B81" s="45"/>
-      <c r="C81" s="84"/>
-      <c r="D81" s="85"/>
-      <c r="E81" s="85"/>
-      <c r="F81" s="85"/>
-      <c r="G81" s="85"/>
-      <c r="H81" s="86"/>
+      <c r="B81" s="41"/>
+      <c r="C81" s="98"/>
+      <c r="D81" s="99"/>
+      <c r="E81" s="99"/>
+      <c r="F81" s="99"/>
+      <c r="G81" s="99"/>
+      <c r="H81" s="100"/>
     </row>
     <row r="82" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B82" s="65" t="s">
-        <v>36</v>
-      </c>
-      <c r="C82" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D82" s="53"/>
-      <c r="E82" s="53"/>
-      <c r="F82" s="53"/>
-      <c r="G82" s="53"/>
-      <c r="H82" s="54"/>
+      <c r="B82" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C82" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="D82" s="47"/>
+      <c r="E82" s="47"/>
+      <c r="F82" s="47"/>
+      <c r="G82" s="47"/>
+      <c r="H82" s="48"/>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B83" s="83"/>
-      <c r="C83" s="67"/>
-      <c r="D83" s="68"/>
-      <c r="E83" s="68"/>
-      <c r="F83" s="68"/>
-      <c r="G83" s="68"/>
-      <c r="H83" s="69"/>
+      <c r="B83" s="97"/>
+      <c r="C83" s="60"/>
+      <c r="D83" s="61"/>
+      <c r="E83" s="61"/>
+      <c r="F83" s="61"/>
+      <c r="G83" s="61"/>
+      <c r="H83" s="62"/>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B84" s="83"/>
-      <c r="C84" s="67"/>
-      <c r="D84" s="68"/>
-      <c r="E84" s="68"/>
-      <c r="F84" s="68"/>
-      <c r="G84" s="68"/>
-      <c r="H84" s="69"/>
+      <c r="B84" s="97"/>
+      <c r="C84" s="60"/>
+      <c r="D84" s="61"/>
+      <c r="E84" s="61"/>
+      <c r="F84" s="61"/>
+      <c r="G84" s="61"/>
+      <c r="H84" s="62"/>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B85" s="83"/>
-      <c r="C85" s="67"/>
-      <c r="D85" s="68"/>
-      <c r="E85" s="68"/>
-      <c r="F85" s="68"/>
-      <c r="G85" s="68"/>
-      <c r="H85" s="69"/>
+      <c r="B85" s="97"/>
+      <c r="C85" s="60"/>
+      <c r="D85" s="61"/>
+      <c r="E85" s="61"/>
+      <c r="F85" s="61"/>
+      <c r="G85" s="61"/>
+      <c r="H85" s="62"/>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B86" s="83"/>
-      <c r="C86" s="67"/>
-      <c r="D86" s="68"/>
-      <c r="E86" s="68"/>
-      <c r="F86" s="68"/>
-      <c r="G86" s="68"/>
-      <c r="H86" s="69"/>
+      <c r="B86" s="97"/>
+      <c r="C86" s="60"/>
+      <c r="D86" s="61"/>
+      <c r="E86" s="61"/>
+      <c r="F86" s="61"/>
+      <c r="G86" s="61"/>
+      <c r="H86" s="62"/>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B87" s="83"/>
-      <c r="C87" s="67"/>
-      <c r="D87" s="68"/>
-      <c r="E87" s="68"/>
-      <c r="F87" s="68"/>
-      <c r="G87" s="68"/>
-      <c r="H87" s="69"/>
+      <c r="B87" s="97"/>
+      <c r="C87" s="60"/>
+      <c r="D87" s="61"/>
+      <c r="E87" s="61"/>
+      <c r="F87" s="61"/>
+      <c r="G87" s="61"/>
+      <c r="H87" s="62"/>
     </row>
     <row r="88" spans="2:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="65" t="s">
-        <v>38</v>
-      </c>
-      <c r="C88" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="D88" s="53"/>
-      <c r="E88" s="53"/>
-      <c r="F88" s="53"/>
-      <c r="G88" s="53"/>
-      <c r="H88" s="54"/>
+      <c r="B88" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="C88" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D88" s="47"/>
+      <c r="E88" s="47"/>
+      <c r="F88" s="47"/>
+      <c r="G88" s="47"/>
+      <c r="H88" s="48"/>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B89" s="83"/>
-      <c r="C89" s="67"/>
-      <c r="D89" s="68"/>
-      <c r="E89" s="68"/>
-      <c r="F89" s="68"/>
-      <c r="G89" s="68"/>
-      <c r="H89" s="69"/>
+      <c r="B89" s="97"/>
+      <c r="C89" s="60"/>
+      <c r="D89" s="61"/>
+      <c r="E89" s="61"/>
+      <c r="F89" s="61"/>
+      <c r="G89" s="61"/>
+      <c r="H89" s="62"/>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B90" s="83"/>
-      <c r="C90" s="67"/>
-      <c r="D90" s="68"/>
-      <c r="E90" s="68"/>
-      <c r="F90" s="68"/>
-      <c r="G90" s="68"/>
-      <c r="H90" s="69"/>
+      <c r="B90" s="97"/>
+      <c r="C90" s="60"/>
+      <c r="D90" s="61"/>
+      <c r="E90" s="61"/>
+      <c r="F90" s="61"/>
+      <c r="G90" s="61"/>
+      <c r="H90" s="62"/>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B91" s="66"/>
-      <c r="C91" s="84"/>
-      <c r="D91" s="85"/>
-      <c r="E91" s="85"/>
-      <c r="F91" s="85"/>
-      <c r="G91" s="85"/>
-      <c r="H91" s="86"/>
+      <c r="B91" s="59"/>
+      <c r="C91" s="98"/>
+      <c r="D91" s="99"/>
+      <c r="E91" s="99"/>
+      <c r="F91" s="99"/>
+      <c r="G91" s="99"/>
+      <c r="H91" s="100"/>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B92" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="C92" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="D92" s="53"/>
-      <c r="E92" s="53"/>
-      <c r="F92" s="53"/>
-      <c r="G92" s="53"/>
-      <c r="H92" s="54"/>
+      <c r="B92" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D92" s="47"/>
+      <c r="E92" s="47"/>
+      <c r="F92" s="47"/>
+      <c r="G92" s="47"/>
+      <c r="H92" s="48"/>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B93" s="66"/>
-      <c r="C93" s="67"/>
-      <c r="D93" s="68"/>
-      <c r="E93" s="68"/>
-      <c r="F93" s="68"/>
-      <c r="G93" s="68"/>
-      <c r="H93" s="69"/>
+      <c r="B93" s="59"/>
+      <c r="C93" s="60"/>
+      <c r="D93" s="61"/>
+      <c r="E93" s="61"/>
+      <c r="F93" s="61"/>
+      <c r="G93" s="61"/>
+      <c r="H93" s="62"/>
     </row>
     <row r="94" spans="2:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B94" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="C94" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D94" s="37"/>
-      <c r="E94" s="37"/>
-      <c r="F94" s="37"/>
-      <c r="G94" s="37"/>
-      <c r="H94" s="38"/>
+      <c r="B94" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C94" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="D94" s="42"/>
+      <c r="E94" s="42"/>
+      <c r="F94" s="42"/>
+      <c r="G94" s="42"/>
+      <c r="H94" s="43"/>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B95" s="45"/>
-      <c r="C95" s="41"/>
-      <c r="D95" s="41"/>
-      <c r="E95" s="41"/>
-      <c r="F95" s="41"/>
-      <c r="G95" s="41"/>
-      <c r="H95" s="42"/>
+      <c r="B95" s="41"/>
+      <c r="C95" s="44"/>
+      <c r="D95" s="44"/>
+      <c r="E95" s="44"/>
+      <c r="F95" s="44"/>
+      <c r="G95" s="44"/>
+      <c r="H95" s="45"/>
     </row>
     <row r="96" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B96" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="C96" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="C96" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D96" s="47"/>
+      <c r="E96" s="47"/>
+      <c r="F96" s="47"/>
+      <c r="G96" s="47"/>
+      <c r="H96" s="48"/>
+    </row>
+    <row r="97" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B97" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C97" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="D97" s="42"/>
+      <c r="E97" s="42"/>
+      <c r="F97" s="42"/>
+      <c r="G97" s="42"/>
+      <c r="H97" s="43"/>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B98" s="41"/>
+      <c r="C98" s="44"/>
+      <c r="D98" s="44"/>
+      <c r="E98" s="44"/>
+      <c r="F98" s="44"/>
+      <c r="G98" s="44"/>
+      <c r="H98" s="45"/>
+    </row>
+    <row r="99" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B99" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D99" s="42"/>
+      <c r="E99" s="42"/>
+      <c r="F99" s="42"/>
+      <c r="G99" s="42"/>
+      <c r="H99" s="43"/>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B100" s="51"/>
+      <c r="C100" s="49"/>
+      <c r="D100" s="49"/>
+      <c r="E100" s="49"/>
+      <c r="F100" s="49"/>
+      <c r="G100" s="49"/>
+      <c r="H100" s="50"/>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B101" s="51"/>
+      <c r="C101" s="49"/>
+      <c r="D101" s="49"/>
+      <c r="E101" s="49"/>
+      <c r="F101" s="49"/>
+      <c r="G101" s="49"/>
+      <c r="H101" s="50"/>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B102" s="51"/>
+      <c r="C102" s="49"/>
+      <c r="D102" s="49"/>
+      <c r="E102" s="49"/>
+      <c r="F102" s="49"/>
+      <c r="G102" s="49"/>
+      <c r="H102" s="50"/>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B103" s="41"/>
+      <c r="C103" s="44"/>
+      <c r="D103" s="44"/>
+      <c r="E103" s="44"/>
+      <c r="F103" s="44"/>
+      <c r="G103" s="44"/>
+      <c r="H103" s="45"/>
+    </row>
+    <row r="104" spans="2:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B104" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C104" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D96" s="53"/>
-      <c r="E96" s="53"/>
-      <c r="F96" s="53"/>
-      <c r="G96" s="53"/>
-      <c r="H96" s="54"/>
-    </row>
-    <row r="97" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B97" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="C97" s="37" t="s">
+      <c r="D104" s="42"/>
+      <c r="E104" s="42"/>
+      <c r="F104" s="42"/>
+      <c r="G104" s="42"/>
+      <c r="H104" s="43"/>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B105" s="51"/>
+      <c r="C105" s="49"/>
+      <c r="D105" s="49"/>
+      <c r="E105" s="49"/>
+      <c r="F105" s="49"/>
+      <c r="G105" s="49"/>
+      <c r="H105" s="50"/>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B106" s="51"/>
+      <c r="C106" s="49"/>
+      <c r="D106" s="49"/>
+      <c r="E106" s="49"/>
+      <c r="F106" s="49"/>
+      <c r="G106" s="49"/>
+      <c r="H106" s="50"/>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B107" s="51"/>
+      <c r="C107" s="49"/>
+      <c r="D107" s="49"/>
+      <c r="E107" s="49"/>
+      <c r="F107" s="49"/>
+      <c r="G107" s="49"/>
+      <c r="H107" s="50"/>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B108" s="51"/>
+      <c r="C108" s="49"/>
+      <c r="D108" s="49"/>
+      <c r="E108" s="49"/>
+      <c r="F108" s="49"/>
+      <c r="G108" s="49"/>
+      <c r="H108" s="50"/>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B109" s="51"/>
+      <c r="C109" s="49"/>
+      <c r="D109" s="49"/>
+      <c r="E109" s="49"/>
+      <c r="F109" s="49"/>
+      <c r="G109" s="49"/>
+      <c r="H109" s="50"/>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B110" s="41"/>
+      <c r="C110" s="44"/>
+      <c r="D110" s="44"/>
+      <c r="E110" s="44"/>
+      <c r="F110" s="44"/>
+      <c r="G110" s="44"/>
+      <c r="H110" s="45"/>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B111" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="D97" s="37"/>
-      <c r="E97" s="37"/>
-      <c r="F97" s="37"/>
-      <c r="G97" s="37"/>
-      <c r="H97" s="38"/>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B98" s="45"/>
-      <c r="C98" s="41"/>
-      <c r="D98" s="41"/>
-      <c r="E98" s="41"/>
-      <c r="F98" s="41"/>
-      <c r="G98" s="41"/>
-      <c r="H98" s="42"/>
-    </row>
-    <row r="99" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B99" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C99" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="D99" s="37"/>
-      <c r="E99" s="37"/>
-      <c r="F99" s="37"/>
-      <c r="G99" s="37"/>
-      <c r="H99" s="38"/>
-    </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B100" s="44"/>
-      <c r="C100" s="39"/>
-      <c r="D100" s="39"/>
-      <c r="E100" s="39"/>
-      <c r="F100" s="39"/>
-      <c r="G100" s="39"/>
-      <c r="H100" s="40"/>
-    </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B101" s="44"/>
-      <c r="C101" s="39"/>
-      <c r="D101" s="39"/>
-      <c r="E101" s="39"/>
-      <c r="F101" s="39"/>
-      <c r="G101" s="39"/>
-      <c r="H101" s="40"/>
-    </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B102" s="44"/>
-      <c r="C102" s="39"/>
-      <c r="D102" s="39"/>
-      <c r="E102" s="39"/>
-      <c r="F102" s="39"/>
-      <c r="G102" s="39"/>
-      <c r="H102" s="40"/>
-    </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B103" s="45"/>
-      <c r="C103" s="41"/>
-      <c r="D103" s="41"/>
-      <c r="E103" s="41"/>
-      <c r="F103" s="41"/>
-      <c r="G103" s="41"/>
-      <c r="H103" s="42"/>
-    </row>
-    <row r="104" spans="2:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B104" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="C104" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="D104" s="37"/>
-      <c r="E104" s="37"/>
-      <c r="F104" s="37"/>
-      <c r="G104" s="37"/>
-      <c r="H104" s="38"/>
-    </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B105" s="44"/>
-      <c r="C105" s="39"/>
-      <c r="D105" s="39"/>
-      <c r="E105" s="39"/>
-      <c r="F105" s="39"/>
-      <c r="G105" s="39"/>
-      <c r="H105" s="40"/>
-    </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B106" s="44"/>
-      <c r="C106" s="39"/>
-      <c r="D106" s="39"/>
-      <c r="E106" s="39"/>
-      <c r="F106" s="39"/>
-      <c r="G106" s="39"/>
-      <c r="H106" s="40"/>
-    </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B107" s="44"/>
-      <c r="C107" s="39"/>
-      <c r="D107" s="39"/>
-      <c r="E107" s="39"/>
-      <c r="F107" s="39"/>
-      <c r="G107" s="39"/>
-      <c r="H107" s="40"/>
-    </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B108" s="44"/>
-      <c r="C108" s="39"/>
-      <c r="D108" s="39"/>
-      <c r="E108" s="39"/>
-      <c r="F108" s="39"/>
-      <c r="G108" s="39"/>
-      <c r="H108" s="40"/>
-    </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B109" s="44"/>
-      <c r="C109" s="39"/>
-      <c r="D109" s="39"/>
-      <c r="E109" s="39"/>
-      <c r="F109" s="39"/>
-      <c r="G109" s="39"/>
-      <c r="H109" s="40"/>
-    </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B110" s="45"/>
-      <c r="C110" s="41"/>
-      <c r="D110" s="41"/>
-      <c r="E110" s="41"/>
-      <c r="F110" s="41"/>
-      <c r="G110" s="41"/>
-      <c r="H110" s="42"/>
-    </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B111" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="C111" s="47"/>
-      <c r="D111" s="47"/>
-      <c r="E111" s="47"/>
-      <c r="F111" s="47"/>
-      <c r="G111" s="47"/>
-      <c r="H111" s="48"/>
+      <c r="C111" s="53"/>
+      <c r="D111" s="53"/>
+      <c r="E111" s="53"/>
+      <c r="F111" s="53"/>
+      <c r="G111" s="53"/>
+      <c r="H111" s="54"/>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B112" s="49"/>
-      <c r="C112" s="50"/>
-      <c r="D112" s="50"/>
-      <c r="E112" s="50"/>
-      <c r="F112" s="50"/>
-      <c r="G112" s="50"/>
-      <c r="H112" s="51"/>
+      <c r="B112" s="55"/>
+      <c r="C112" s="56"/>
+      <c r="D112" s="56"/>
+      <c r="E112" s="56"/>
+      <c r="F112" s="56"/>
+      <c r="G112" s="56"/>
+      <c r="H112" s="57"/>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B113" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C113" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D113" s="37"/>
+      <c r="E113" s="37"/>
+      <c r="F113" s="37"/>
+      <c r="G113" s="37"/>
+      <c r="H113" s="38"/>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B114" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C114" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="D114" s="37"/>
+      <c r="E114" s="37"/>
+      <c r="F114" s="37"/>
+      <c r="G114" s="37"/>
+      <c r="H114" s="38"/>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B115" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C113" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="D113" s="35"/>
-      <c r="E113" s="35"/>
-      <c r="F113" s="35"/>
-      <c r="G113" s="35"/>
-      <c r="H113" s="36"/>
-    </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B114" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C114" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="D114" s="35"/>
-      <c r="E114" s="35"/>
-      <c r="F114" s="35"/>
-      <c r="G114" s="35"/>
-      <c r="H114" s="36"/>
-    </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B115" s="19" t="s">
-        <v>27</v>
-      </c>
+      <c r="C115" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="D115" s="37"/>
+      <c r="E115" s="37"/>
+      <c r="F115" s="37"/>
+      <c r="G115" s="37"/>
+      <c r="H115" s="38"/>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B116" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B117" s="9" t="s">
-        <v>46</v>
-      </c>
+      <c r="B116" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C116" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="D116" s="37"/>
+      <c r="E116" s="37"/>
+      <c r="F116" s="37"/>
+      <c r="G116" s="37"/>
+      <c r="H116" s="38"/>
+    </row>
+    <row r="117" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B117" s="91" t="s">
+        <v>43</v>
+      </c>
+      <c r="C117" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="D117" s="42"/>
+      <c r="E117" s="42"/>
+      <c r="F117" s="42"/>
+      <c r="G117" s="42"/>
+      <c r="H117" s="43"/>
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B118" s="92"/>
+      <c r="C118" s="49"/>
+      <c r="D118" s="49"/>
+      <c r="E118" s="49"/>
+      <c r="F118" s="49"/>
+      <c r="G118" s="49"/>
+      <c r="H118" s="50"/>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B119" s="92"/>
+      <c r="C119" s="49"/>
+      <c r="D119" s="49"/>
+      <c r="E119" s="49"/>
+      <c r="F119" s="49"/>
+      <c r="G119" s="49"/>
+      <c r="H119" s="50"/>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B120" s="93"/>
+      <c r="C120" s="44"/>
+      <c r="D120" s="44"/>
+      <c r="E120" s="44"/>
+      <c r="F120" s="44"/>
+      <c r="G120" s="44"/>
+      <c r="H120" s="45"/>
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B121" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C121" s="89" t="s">
+        <v>73</v>
+      </c>
+      <c r="D121" s="89"/>
+      <c r="E121" s="89"/>
+      <c r="F121" s="89"/>
+      <c r="G121" s="89"/>
+      <c r="H121" s="90"/>
     </row>
   </sheetData>
-  <mergeCells count="58">
-    <mergeCell ref="B63:B66"/>
+  <mergeCells count="63">
+    <mergeCell ref="C121:H121"/>
+    <mergeCell ref="C113:H113"/>
+    <mergeCell ref="B117:B120"/>
+    <mergeCell ref="C117:H120"/>
+    <mergeCell ref="B50:H51"/>
+    <mergeCell ref="B61:H62"/>
+    <mergeCell ref="B56:H57"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="C88:H91"/>
+    <mergeCell ref="B52:H55"/>
+    <mergeCell ref="C67:H67"/>
+    <mergeCell ref="C75:H81"/>
+    <mergeCell ref="B75:B81"/>
+    <mergeCell ref="C82:H87"/>
+    <mergeCell ref="B82:B87"/>
+    <mergeCell ref="C71:H74"/>
+    <mergeCell ref="C58:H58"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="C68:H70"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="C59:H59"/>
+    <mergeCell ref="C60:H60"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="C63:H66"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="C10:C16"/>
     <mergeCell ref="F26:F30"/>
@@ -2610,38 +2926,11 @@
     <mergeCell ref="C26:C30"/>
     <mergeCell ref="C20:C24"/>
     <mergeCell ref="C32:C37"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="C92:H93"/>
-    <mergeCell ref="C68:H70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="C59:H59"/>
-    <mergeCell ref="C60:H60"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="C58:H58"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="C115:H115"/>
+    <mergeCell ref="C116:H116"/>
+    <mergeCell ref="B63:B66"/>
     <mergeCell ref="B94:B95"/>
     <mergeCell ref="C94:H95"/>
-    <mergeCell ref="B50:H51"/>
-    <mergeCell ref="B61:H62"/>
-    <mergeCell ref="B56:H57"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="C88:H91"/>
-    <mergeCell ref="B52:H55"/>
-    <mergeCell ref="C67:H67"/>
-    <mergeCell ref="C75:H81"/>
-    <mergeCell ref="B75:B81"/>
-    <mergeCell ref="C82:H87"/>
-    <mergeCell ref="B82:B87"/>
-    <mergeCell ref="C71:H74"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="C63:H66"/>
     <mergeCell ref="C96:H96"/>
     <mergeCell ref="B97:B98"/>
     <mergeCell ref="C97:H98"/>
@@ -2651,7 +2940,8 @@
     <mergeCell ref="C104:H110"/>
     <mergeCell ref="B104:B110"/>
     <mergeCell ref="B111:H112"/>
-    <mergeCell ref="C113:H113"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="C92:H93"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>